<commit_message>
cambio en escaleta CN_08_08_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion08/Escaleta CN_08_08_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion08/Escaleta CN_08_08_CO.xlsx
@@ -1048,16 +1048,34 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1097,24 +1115,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1424,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,94 +1455,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="66" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="72" t="s">
+      <c r="M1" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="72"/>
-      <c r="O1" s="60" t="s">
+      <c r="N1" s="78"/>
+      <c r="O1" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="60" t="s">
+      <c r="P1" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="75" t="s">
+      <c r="Q1" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="79" t="s">
+      <c r="R1" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="75" t="s">
+      <c r="S1" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="77" t="s">
+      <c r="T1" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="75" t="s">
+      <c r="U1" s="60" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="14" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="65"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="67"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="73"/>
       <c r="M2" s="15" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="76"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="76"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="61"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -4941,12 +4941,6 @@
   </sheetData>
   <autoFilter ref="A2:U54"/>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4961,6 +4955,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O42" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion escaleta y guion CN_08_08_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion08/Escaleta CN_08_08_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion08/Escaleta CN_08_08_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOSHIBA 1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOSHIBA 1\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado08\guion08\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="237">
   <si>
     <t>Asignatura</t>
   </si>
@@ -444,9 +444,6 @@
     <t>Las curvas de sobrevivencia</t>
   </si>
   <si>
-    <t>Recurso M101A-05</t>
-  </si>
-  <si>
     <t xml:space="preserve">Refuerza tu aprendizaje: La demografía humana </t>
   </si>
   <si>
@@ -510,9 +507,6 @@
     <t>Recurso F8-01</t>
   </si>
   <si>
-    <t>Recurso M5A-03</t>
-  </si>
-  <si>
     <t>La dispersión de la especie humana por planeta Tierra</t>
   </si>
   <si>
@@ -525,9 +519,6 @@
     <t>Proyecto: determinación de la densidad de una población de cochinillas</t>
   </si>
   <si>
-    <t>Cambios en el tamaño de la población</t>
-  </si>
-  <si>
     <t>Actividad que consolida conocimientos sobre Cambios en el tamaño de la población</t>
   </si>
   <si>
@@ -537,9 +528,6 @@
     <t>Recurso F13-01</t>
   </si>
   <si>
-    <t>Recurso M101A-06</t>
-  </si>
-  <si>
     <t>Recurso M10B-01</t>
   </si>
   <si>
@@ -600,9 +588,6 @@
     <t>Las poblaciones naturales</t>
   </si>
   <si>
-    <t>Tamaño y densidad de una población</t>
-  </si>
-  <si>
     <t>¿Qué es la distribución espacial?</t>
   </si>
   <si>
@@ -612,9 +597,6 @@
     <t>La distribución de edades</t>
   </si>
   <si>
-    <t>Crecimiento de las poblaciones naturales</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Parámetros que determinan la densidad de las poblaciones</t>
   </si>
   <si>
@@ -636,12 +618,6 @@
     <t>¿Qué son las estrategias de vida?</t>
   </si>
   <si>
-    <t>La distribución de  sexos</t>
-  </si>
-  <si>
-    <t>Parámetros básicos que determinan la densidad de las poblaciones</t>
-  </si>
-  <si>
     <t>Interactivo sobre la dinámica de las poblaciones</t>
   </si>
   <si>
@@ -672,18 +648,12 @@
     <t>Refuerza tu aprendizaje: Evolución y dispersión de los homínidos</t>
   </si>
   <si>
-    <t>Evolución de las poblaciones humanas</t>
-  </si>
-  <si>
     <t>¿Cómo pobló el planeta la especie humana?</t>
   </si>
   <si>
     <t>¿Qué es la demografía humana?</t>
   </si>
   <si>
-    <t xml:space="preserve">¿Qué estudia la demografía? </t>
-  </si>
-  <si>
     <t>¿Cómo ha crecido la población humana a través del tiempo?</t>
   </si>
   <si>
@@ -733,6 +703,39 @@
   </si>
   <si>
     <t>Recurso F13-04</t>
+  </si>
+  <si>
+    <t>Estudios demográficos</t>
+  </si>
+  <si>
+    <t>¿Qué es la densidad de una población natural?</t>
+  </si>
+  <si>
+    <t>Los parámetros que caracterizan a las poblaciones</t>
+  </si>
+  <si>
+    <t>La densidad de una poblacion</t>
+  </si>
+  <si>
+    <t>La distribución de sexos en una población</t>
+  </si>
+  <si>
+    <t>El crecimiento de las poblaciones naturales</t>
+  </si>
+  <si>
+    <t>Las poblaciones humanas</t>
+  </si>
+  <si>
+    <t>Recurso M101A-02</t>
+  </si>
+  <si>
+    <t>Recurso M101A-04</t>
+  </si>
+  <si>
+    <t>Recurso M8A-01</t>
+  </si>
+  <si>
+    <t>Recurso F4-01</t>
   </si>
 </sst>
 </file>
@@ -918,7 +921,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1019,28 +1022,29 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1050,12 +1054,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1076,13 +1074,19 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1390,9 +1394,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U267"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T40" sqref="T40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,94 +1426,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="11" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="I1" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="75" t="s">
+      <c r="J1" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="73" t="s">
+      <c r="K1" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="71" t="s">
+      <c r="L1" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="68" t="s">
+      <c r="M1" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="68"/>
-      <c r="O1" s="58" t="s">
+      <c r="N1" s="69"/>
+      <c r="O1" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="58" t="s">
+      <c r="P1" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="60" t="s">
+      <c r="Q1" s="76" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="R1" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="60" t="s">
+      <c r="S1" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="62" t="s">
+      <c r="T1" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="60" t="s">
+      <c r="U1" s="76" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="11" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="70"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="72"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="71"/>
       <c r="M2" s="12" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="61"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="77"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -1519,10 +1523,10 @@
         <v>123</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="17"/>
@@ -1550,13 +1554,13 @@
         <v>123</v>
       </c>
       <c r="C4" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>227</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>191</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="18"/>
@@ -1583,13 +1587,13 @@
         <v>123</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F5" s="53" t="s">
         <v>125</v>
@@ -1618,13 +1622,13 @@
         <v>123</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>124</v>
@@ -1653,19 +1657,19 @@
         <v>123</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F7" s="53" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="H7" s="47">
         <v>1</v>
@@ -1674,7 +1678,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="K7" s="21" t="s">
         <v>20</v>
@@ -1697,13 +1701,13 @@
         <v>128</v>
       </c>
       <c r="S7" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="T7" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="T7" s="35" t="s">
+      <c r="U7" s="34" t="s">
         <v>150</v>
-      </c>
-      <c r="U7" s="34" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1714,19 +1718,19 @@
         <v>123</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G8" s="54" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H8" s="47">
         <v>2</v>
@@ -1735,7 +1739,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>20</v>
@@ -1761,7 +1765,7 @@
         <v>129</v>
       </c>
       <c r="T8" s="35" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="U8" s="34" t="s">
         <v>131</v>
@@ -1774,18 +1778,18 @@
       <c r="B9" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="79" t="s">
-        <v>227</v>
+      <c r="C9" s="58" t="s">
+        <v>217</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>126</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H9" s="48">
         <v>3</v>
@@ -1794,7 +1798,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K9" s="29" t="s">
         <v>20</v>
@@ -1834,10 +1838,10 @@
         <v>123</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
       <c r="E10" s="46"/>
       <c r="F10" s="17"/>
@@ -1865,13 +1869,13 @@
         <v>123</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="18"/>
@@ -1898,13 +1902,13 @@
         <v>123</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>132</v>
@@ -1933,13 +1937,13 @@
         <v>123</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>133</v>
@@ -1968,13 +1972,13 @@
         <v>123</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
       <c r="F14" s="17" t="s">
         <v>134</v>
@@ -2003,17 +2007,15 @@
         <v>123</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>204</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>194</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="F15" s="17"/>
       <c r="G15" s="18"/>
       <c r="H15" s="47"/>
       <c r="I15" s="19"/>
@@ -2038,19 +2040,17 @@
         <v>123</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>204</v>
-      </c>
-      <c r="F16" s="53" t="s">
-        <v>203</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="F16" s="53"/>
       <c r="G16" s="18" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H16" s="47">
         <v>4</v>
@@ -2059,7 +2059,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="56" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="K16" s="21" t="s">
         <v>20</v>
@@ -2082,13 +2082,13 @@
         <v>128</v>
       </c>
       <c r="S16" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T16" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U16" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:21" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2099,19 +2099,17 @@
         <v>123</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>204</v>
-      </c>
-      <c r="F17" s="53" t="s">
-        <v>203</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="F17" s="53"/>
       <c r="G17" s="55" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H17" s="47">
         <v>5</v>
@@ -2120,7 +2118,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="K17" s="21" t="s">
         <v>20</v>
@@ -2146,7 +2144,7 @@
         <v>129</v>
       </c>
       <c r="T17" s="35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U17" s="34" t="s">
         <v>131</v>
@@ -2159,18 +2157,18 @@
       <c r="B18" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="79" t="s">
-        <v>227</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>166</v>
+      <c r="C18" s="58" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18" s="80" t="s">
+        <v>228</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>126</v>
       </c>
       <c r="F18" s="53"/>
       <c r="G18" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="H18" s="48">
         <v>6</v>
@@ -2179,7 +2177,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K18" s="29" t="s">
         <v>20</v>
@@ -2205,7 +2203,7 @@
         <v>129</v>
       </c>
       <c r="T18" s="9" t="s">
-        <v>135</v>
+        <v>233</v>
       </c>
       <c r="U18" s="8" t="s">
         <v>131</v>
@@ -2219,10 +2217,10 @@
         <v>123</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="E19" s="36"/>
       <c r="F19" s="17"/>
@@ -2250,17 +2248,17 @@
         <v>123</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F20" s="53"/>
       <c r="G20" s="54" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H20" s="47"/>
       <c r="I20" s="19"/>
@@ -2285,17 +2283,17 @@
         <v>123</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="18" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="H21" s="47">
         <v>7</v>
@@ -2304,7 +2302,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K21" s="21" t="s">
         <v>20</v>
@@ -2330,7 +2328,7 @@
         <v>129</v>
       </c>
       <c r="T21" s="35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U21" s="34" t="s">
         <v>131</v>
@@ -2344,13 +2342,13 @@
         <v>123</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="E22" s="36" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>136</v>
@@ -2379,13 +2377,13 @@
         <v>123</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="E23" s="36" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>137</v>
@@ -2400,7 +2398,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K23" s="21" t="s">
         <v>20</v>
@@ -2423,13 +2421,13 @@
         <v>128</v>
       </c>
       <c r="S23" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T23" s="35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="U23" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2440,19 +2438,19 @@
         <v>123</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="E24" s="36" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>137</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H24" s="50">
         <v>9</v>
@@ -2461,7 +2459,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="40" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="K24" s="41" t="s">
         <v>20</v>
@@ -2487,7 +2485,7 @@
         <v>129</v>
       </c>
       <c r="T24" s="25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="U24" s="24" t="s">
         <v>131</v>
@@ -2500,18 +2498,18 @@
       <c r="B25" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="79" t="s">
-        <v>227</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>202</v>
+      <c r="C25" s="58" t="s">
+        <v>217</v>
+      </c>
+      <c r="D25" s="80" t="s">
+        <v>231</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>126</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H25" s="48">
         <v>10</v>
@@ -2520,7 +2518,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K25" s="29" t="s">
         <v>20</v>
@@ -2546,7 +2544,7 @@
         <v>129</v>
       </c>
       <c r="T25" s="9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="U25" s="8" t="s">
         <v>131</v>
@@ -2560,15 +2558,15 @@
         <v>123</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E26" s="52"/>
       <c r="F26" s="17"/>
       <c r="G26" s="54" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H26" s="47">
         <v>11</v>
@@ -2577,18 +2575,18 @@
         <v>20</v>
       </c>
       <c r="J26" s="56" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>19</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M26" s="23"/>
       <c r="N26" s="23"/>
       <c r="O26" s="45" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="P26" s="57" t="s">
         <v>19</v>
@@ -2607,17 +2605,17 @@
         <v>123</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E27" s="52" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="H27" s="47">
         <v>12</v>
@@ -2626,7 +2624,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>20</v>
@@ -2652,7 +2650,7 @@
         <v>129</v>
       </c>
       <c r="T27" s="25" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="U27" s="24" t="s">
         <v>131</v>
@@ -2666,17 +2664,17 @@
         <v>123</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="54" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H28" s="47">
         <v>13</v>
@@ -2685,7 +2683,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="20" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>20</v>
@@ -2708,13 +2706,13 @@
         <v>128</v>
       </c>
       <c r="S28" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T28" s="25" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="U28" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2725,17 +2723,17 @@
         <v>123</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="54" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H29" s="47">
         <v>14</v>
@@ -2744,7 +2742,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>20</v>
@@ -2770,7 +2768,7 @@
         <v>129</v>
       </c>
       <c r="T29" s="25" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="U29" s="24" t="s">
         <v>131</v>
@@ -2783,18 +2781,18 @@
       <c r="B30" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C30" s="79" t="s">
-        <v>227</v>
+      <c r="C30" s="58" t="s">
+        <v>217</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>126</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="6" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="H30" s="48">
         <v>15</v>
@@ -2803,7 +2801,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="K30" s="29" t="s">
         <v>19</v>
@@ -2829,7 +2827,7 @@
         <v>129</v>
       </c>
       <c r="T30" s="9" t="s">
-        <v>170</v>
+        <v>234</v>
       </c>
       <c r="U30" s="8" t="s">
         <v>131</v>
@@ -2843,10 +2841,10 @@
         <v>123</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D31" s="51" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="17"/>
@@ -2874,20 +2872,20 @@
         <v>123</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D32" s="51" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="18"/>
       <c r="H32" s="47"/>
       <c r="I32" s="19"/>
       <c r="J32" s="56" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="K32" s="21"/>
       <c r="L32" s="22"/>
@@ -2909,13 +2907,13 @@
         <v>123</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D33" s="51" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="E33" s="52" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="18"/>
@@ -2942,13 +2940,13 @@
         <v>123</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D34" s="51" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
@@ -2975,17 +2973,17 @@
         <v>123</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D35" s="51" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="54" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H35" s="47">
         <v>16</v>
@@ -2994,7 +2992,7 @@
         <v>19</v>
       </c>
       <c r="J35" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K35" s="21" t="s">
         <v>20</v>
@@ -3010,20 +3008,20 @@
       <c r="P35" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="Q35" s="34">
+      <c r="Q35" s="24">
         <v>6</v>
       </c>
-      <c r="R35" s="34" t="s">
+      <c r="R35" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="S35" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="T35" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="U35" s="34" t="s">
-        <v>131</v>
+      <c r="S35" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="T35" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="U35" s="24" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3034,17 +3032,17 @@
         <v>123</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D36" s="51" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="18" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="H36" s="47">
         <v>17</v>
@@ -3053,7 +3051,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="20" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="K36" s="21" t="s">
         <v>20</v>
@@ -3069,11 +3067,21 @@
       <c r="P36" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24"/>
-      <c r="S36" s="24"/>
-      <c r="T36" s="25"/>
-      <c r="U36" s="24"/>
+      <c r="Q36" s="34">
+        <v>6</v>
+      </c>
+      <c r="R36" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="S36" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="T36" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="U36" s="34" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
@@ -3082,20 +3090,20 @@
       <c r="B37" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="79" t="s">
-        <v>227</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>206</v>
+      <c r="C37" s="58" t="s">
+        <v>217</v>
+      </c>
+      <c r="D37" s="51" t="s">
+        <v>232</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>126</v>
       </c>
       <c r="F37" s="53" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H37" s="48">
         <v>18</v>
@@ -3104,7 +3112,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K37" s="29" t="s">
         <v>20</v>
@@ -3120,11 +3128,21 @@
       <c r="P37" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q37" s="24"/>
-      <c r="R37" s="24"/>
-      <c r="S37" s="24"/>
-      <c r="T37" s="25"/>
-      <c r="U37" s="24"/>
+      <c r="Q37" s="8">
+        <v>6</v>
+      </c>
+      <c r="R37" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="S37" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="T37" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="U37" s="8" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
@@ -3134,15 +3152,15 @@
         <v>123</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="17"/>
       <c r="G38" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H38" s="47">
         <v>19</v>
@@ -3151,7 +3169,7 @@
         <v>19</v>
       </c>
       <c r="J38" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K38" s="21" t="s">
         <v>20</v>
@@ -3174,13 +3192,13 @@
         <v>128</v>
       </c>
       <c r="S38" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T38" s="35" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="U38" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3191,15 +3209,15 @@
         <v>123</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="17"/>
       <c r="G39" s="18" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H39" s="47">
         <v>20</v>
@@ -3208,7 +3226,7 @@
         <v>19</v>
       </c>
       <c r="J39" s="20" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K39" s="21" t="s">
         <v>20</v>
@@ -3221,7 +3239,7 @@
       </c>
       <c r="N39" s="23"/>
       <c r="O39" s="45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P39" s="47" t="s">
         <v>20</v>
@@ -3233,13 +3251,13 @@
         <v>128</v>
       </c>
       <c r="S39" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T39" s="35" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="U39" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3250,15 +3268,15 @@
         <v>123</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="17"/>
       <c r="G40" s="18" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="H40" s="47">
         <v>21</v>
@@ -3284,13 +3302,13 @@
       </c>
       <c r="R40" s="34"/>
       <c r="S40" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T40" s="35" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="U40" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3301,15 +3319,15 @@
         <v>123</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E41" s="14"/>
       <c r="F41" s="17"/>
       <c r="G41" s="18" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="H41" s="47">
         <v>22</v>
@@ -3335,13 +3353,13 @@
       </c>
       <c r="R41" s="34"/>
       <c r="S41" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T41" s="35" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="U41" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3352,15 +3370,15 @@
         <v>123</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="17"/>
       <c r="G42" s="18" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="H42" s="47">
         <v>23</v>
@@ -3386,13 +3404,13 @@
       </c>
       <c r="R42" s="34"/>
       <c r="S42" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T42" s="35" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="U42" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:21" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3402,11 +3420,11 @@
       <c r="B43" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C43" s="79" t="s">
-        <v>227</v>
+      <c r="C43" s="58" t="s">
+        <v>217</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="5"/>
@@ -3418,7 +3436,7 @@
       </c>
       <c r="I43" s="28"/>
       <c r="J43" s="7" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="K43" s="29" t="s">
         <v>20</v>
@@ -3443,16 +3461,16 @@
       <c r="B44" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C44" s="79" t="s">
-        <v>227</v>
+      <c r="C44" s="58" t="s">
+        <v>217</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="5"/>
       <c r="G44" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H44" s="48">
         <v>25</v>
@@ -3461,7 +3479,7 @@
         <v>20</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K44" s="29" t="s">
         <v>20</v>
@@ -3487,7 +3505,7 @@
         <v>129</v>
       </c>
       <c r="T44" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="U44" s="8" t="s">
         <v>131</v>
@@ -3500,16 +3518,16 @@
       <c r="B45" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C45" s="79" t="s">
-        <v>227</v>
+      <c r="C45" s="58" t="s">
+        <v>217</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="5"/>
       <c r="G45" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H45" s="48">
         <v>26</v>
@@ -3518,7 +3536,7 @@
         <v>20</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K45" s="29" t="s">
         <v>20</v>
@@ -3544,7 +3562,7 @@
         <v>129</v>
       </c>
       <c r="T45" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="U45" s="8" t="s">
         <v>131</v>
@@ -4098,11 +4116,12 @@
   </sheetData>
   <autoFilter ref="A2:U45"/>
   <mergeCells count="20">
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="M1:N1"/>
@@ -4112,12 +4131,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Actualizacion de escaleta CN_08_08_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion08/Escaleta CN_08_08_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion08/Escaleta CN_08_08_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpgarcia\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado08\guion08\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOSHIBA 1\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado08\guion08\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="240">
   <si>
     <t>Asignatura</t>
   </si>
@@ -453,9 +453,6 @@
     <t>Competencias</t>
   </si>
   <si>
-    <t>Determinación de la densidad de una población de cochinillas por medio del método de captura y recaptura</t>
-  </si>
-  <si>
     <t>Fin de unidad</t>
   </si>
   <si>
@@ -549,9 +546,6 @@
     <t>Interactivo en el que se muestran gráficas y ejemplos sobre las curvas de sobrevivencia</t>
   </si>
   <si>
-    <t>Presentación en la que se describen, en orden cronológico, las diferentes etapas de dispersión de la especie humana por el planeta Tierra</t>
-  </si>
-  <si>
     <t>La evolución de la especie humana</t>
   </si>
   <si>
@@ -561,9 +555,6 @@
     <t>La pirámide poblacional de Colombia</t>
   </si>
   <si>
-    <t>Elaboración y análisis de la pirámide poblacional de Colombia fundamentada en datos obtenidos del DANE</t>
-  </si>
-  <si>
     <t>Banco de actividades: Las poblaciones</t>
   </si>
   <si>
@@ -736,6 +727,24 @@
   </si>
   <si>
     <t>Recurso F4-01</t>
+  </si>
+  <si>
+    <t>Actividad que guía el trabajo para la determinación de la densidad de una población de cochinillas por medio del método de captura y recaptura</t>
+  </si>
+  <si>
+    <t>interactivo que presenta una descripción, en orden cronológico,de las diferentes etapas de dispersión de la especie humana por el planeta Tierra</t>
+  </si>
+  <si>
+    <t>Actividad en la que se elabora y analiza la pirámide poblacional de Colombia fundamentada en datos obtenidos del DANE</t>
+  </si>
+  <si>
+    <t>Actividad en la que se estudia un evento de la población de langostas</t>
+  </si>
+  <si>
+    <t>Actividad que permite relacionar una población de primates con su estrategia reproductiva</t>
+  </si>
+  <si>
+    <t>Actividad que estudia la distribución por edad en las poblaciones en los países en desarrollo</t>
   </si>
 </sst>
 </file>
@@ -1394,9 +1403,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L44" sqref="L44"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,10 +1532,10 @@
         <v>123</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="17"/>
@@ -1554,13 +1563,13 @@
         <v>123</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="18"/>
@@ -1587,13 +1596,13 @@
         <v>123</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F5" s="53" t="s">
         <v>125</v>
@@ -1622,13 +1631,13 @@
         <v>123</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>124</v>
@@ -1657,19 +1666,19 @@
         <v>123</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F7" s="53" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H7" s="47">
         <v>1</v>
@@ -1678,7 +1687,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K7" s="21" t="s">
         <v>20</v>
@@ -1701,13 +1710,13 @@
         <v>128</v>
       </c>
       <c r="S7" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="T7" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="T7" s="35" t="s">
+      <c r="U7" s="34" t="s">
         <v>149</v>
-      </c>
-      <c r="U7" s="34" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1718,19 +1727,19 @@
         <v>123</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G8" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H8" s="47">
         <v>2</v>
@@ -1739,7 +1748,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>20</v>
@@ -1765,7 +1774,7 @@
         <v>129</v>
       </c>
       <c r="T8" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U8" s="34" t="s">
         <v>131</v>
@@ -1779,17 +1788,17 @@
         <v>127</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>126</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H9" s="48">
         <v>3</v>
@@ -1798,7 +1807,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K9" s="29" t="s">
         <v>20</v>
@@ -1838,10 +1847,10 @@
         <v>123</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E10" s="46"/>
       <c r="F10" s="17"/>
@@ -1869,13 +1878,13 @@
         <v>123</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="18"/>
@@ -1902,13 +1911,13 @@
         <v>123</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>132</v>
@@ -1937,13 +1946,13 @@
         <v>123</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>133</v>
@@ -1972,13 +1981,13 @@
         <v>123</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F14" s="17" t="s">
         <v>134</v>
@@ -2007,13 +2016,13 @@
         <v>123</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="18"/>
@@ -2040,17 +2049,17 @@
         <v>123</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F16" s="53"/>
       <c r="G16" s="18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H16" s="47">
         <v>4</v>
@@ -2059,7 +2068,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="56" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K16" s="21" t="s">
         <v>20</v>
@@ -2082,13 +2091,13 @@
         <v>128</v>
       </c>
       <c r="S16" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T16" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U16" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:21" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2099,17 +2108,17 @@
         <v>123</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F17" s="53"/>
       <c r="G17" s="55" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H17" s="47">
         <v>5</v>
@@ -2118,7 +2127,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K17" s="21" t="s">
         <v>20</v>
@@ -2144,7 +2153,7 @@
         <v>129</v>
       </c>
       <c r="T17" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U17" s="34" t="s">
         <v>131</v>
@@ -2158,17 +2167,17 @@
         <v>127</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D18" s="59" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>126</v>
       </c>
       <c r="F18" s="53"/>
       <c r="G18" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H18" s="48">
         <v>6</v>
@@ -2177,7 +2186,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K18" s="29" t="s">
         <v>20</v>
@@ -2203,7 +2212,7 @@
         <v>129</v>
       </c>
       <c r="T18" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="U18" s="8" t="s">
         <v>131</v>
@@ -2217,10 +2226,10 @@
         <v>123</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E19" s="36"/>
       <c r="F19" s="17"/>
@@ -2248,17 +2257,17 @@
         <v>123</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F20" s="53"/>
       <c r="G20" s="54" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H20" s="47"/>
       <c r="I20" s="19"/>
@@ -2283,17 +2292,17 @@
         <v>123</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="18" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H21" s="47">
         <v>7</v>
@@ -2302,7 +2311,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K21" s="21" t="s">
         <v>20</v>
@@ -2328,7 +2337,7 @@
         <v>129</v>
       </c>
       <c r="T21" s="35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U21" s="34" t="s">
         <v>131</v>
@@ -2342,13 +2351,13 @@
         <v>123</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E22" s="36" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>136</v>
@@ -2377,13 +2386,13 @@
         <v>123</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E23" s="36" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>137</v>
@@ -2398,7 +2407,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K23" s="21" t="s">
         <v>20</v>
@@ -2421,13 +2430,13 @@
         <v>128</v>
       </c>
       <c r="S23" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T23" s="35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="U23" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2438,19 +2447,19 @@
         <v>123</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E24" s="36" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>137</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H24" s="50">
         <v>9</v>
@@ -2459,7 +2468,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="40" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="K24" s="41" t="s">
         <v>20</v>
@@ -2485,7 +2494,7 @@
         <v>129</v>
       </c>
       <c r="T24" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U24" s="24" t="s">
         <v>131</v>
@@ -2499,17 +2508,17 @@
         <v>123</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D25" s="59" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>126</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H25" s="48">
         <v>10</v>
@@ -2518,7 +2527,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K25" s="29" t="s">
         <v>20</v>
@@ -2558,15 +2567,15 @@
         <v>123</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E26" s="52"/>
       <c r="F26" s="17"/>
       <c r="G26" s="54" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H26" s="47">
         <v>11</v>
@@ -2575,18 +2584,18 @@
         <v>20</v>
       </c>
       <c r="J26" s="56" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>19</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="M26" s="23"/>
       <c r="N26" s="23"/>
       <c r="O26" s="45" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="P26" s="57" t="s">
         <v>19</v>
@@ -2605,17 +2614,17 @@
         <v>123</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E27" s="52" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H27" s="47">
         <v>12</v>
@@ -2624,7 +2633,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>20</v>
@@ -2650,7 +2659,7 @@
         <v>129</v>
       </c>
       <c r="T27" s="25" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="U27" s="24" t="s">
         <v>131</v>
@@ -2664,17 +2673,17 @@
         <v>123</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H28" s="47">
         <v>13</v>
@@ -2683,7 +2692,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="20" t="s">
-        <v>174</v>
+        <v>235</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>20</v>
@@ -2706,13 +2715,13 @@
         <v>128</v>
       </c>
       <c r="S28" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T28" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U28" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2723,17 +2732,17 @@
         <v>123</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="54" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H29" s="47">
         <v>14</v>
@@ -2742,7 +2751,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>20</v>
@@ -2768,7 +2777,7 @@
         <v>129</v>
       </c>
       <c r="T29" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U29" s="24" t="s">
         <v>131</v>
@@ -2782,17 +2791,17 @@
         <v>127</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>126</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H30" s="48">
         <v>15</v>
@@ -2801,7 +2810,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K30" s="29" t="s">
         <v>19</v>
@@ -2827,7 +2836,7 @@
         <v>129</v>
       </c>
       <c r="T30" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="U30" s="8" t="s">
         <v>131</v>
@@ -2841,10 +2850,10 @@
         <v>123</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D31" s="51" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="17"/>
@@ -2872,20 +2881,20 @@
         <v>123</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D32" s="51" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="18"/>
       <c r="H32" s="47"/>
       <c r="I32" s="19"/>
       <c r="J32" s="56" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K32" s="21"/>
       <c r="L32" s="22"/>
@@ -2907,13 +2916,13 @@
         <v>123</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D33" s="51" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E33" s="52" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="18"/>
@@ -2940,13 +2949,13 @@
         <v>123</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D34" s="51" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
@@ -2973,17 +2982,17 @@
         <v>123</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D35" s="51" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="54" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H35" s="47">
         <v>16</v>
@@ -2992,7 +3001,7 @@
         <v>19</v>
       </c>
       <c r="J35" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K35" s="21" t="s">
         <v>20</v>
@@ -3015,13 +3024,13 @@
         <v>128</v>
       </c>
       <c r="S35" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T35" s="25" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="U35" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3032,17 +3041,17 @@
         <v>123</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D36" s="51" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="18" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H36" s="47">
         <v>17</v>
@@ -3051,7 +3060,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="20" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K36" s="21" t="s">
         <v>20</v>
@@ -3077,7 +3086,7 @@
         <v>129</v>
       </c>
       <c r="T36" s="35" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="U36" s="34" t="s">
         <v>131</v>
@@ -3091,16 +3100,16 @@
         <v>127</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D37" s="51" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>126</v>
       </c>
       <c r="F37" s="53" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>139</v>
@@ -3138,7 +3147,7 @@
         <v>129</v>
       </c>
       <c r="T37" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="U37" s="8" t="s">
         <v>131</v>
@@ -3152,7 +3161,7 @@
         <v>123</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>141</v>
@@ -3160,7 +3169,7 @@
       <c r="E38" s="14"/>
       <c r="F38" s="17"/>
       <c r="G38" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H38" s="47">
         <v>19</v>
@@ -3169,7 +3178,7 @@
         <v>19</v>
       </c>
       <c r="J38" s="20" t="s">
-        <v>142</v>
+        <v>234</v>
       </c>
       <c r="K38" s="21" t="s">
         <v>20</v>
@@ -3178,7 +3187,7 @@
         <v>5</v>
       </c>
       <c r="M38" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N38" s="23"/>
       <c r="O38" s="17"/>
@@ -3192,13 +3201,13 @@
         <v>128</v>
       </c>
       <c r="S38" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T38" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U38" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3209,7 +3218,7 @@
         <v>123</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D39" s="16" t="s">
         <v>141</v>
@@ -3217,7 +3226,7 @@
       <c r="E39" s="14"/>
       <c r="F39" s="17"/>
       <c r="G39" s="18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H39" s="47">
         <v>20</v>
@@ -3226,7 +3235,7 @@
         <v>19</v>
       </c>
       <c r="J39" s="20" t="s">
-        <v>178</v>
+        <v>236</v>
       </c>
       <c r="K39" s="21" t="s">
         <v>20</v>
@@ -3234,12 +3243,12 @@
       <c r="L39" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M39" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N39" s="23"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="O39" s="45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P39" s="47" t="s">
         <v>20</v>
@@ -3251,13 +3260,13 @@
         <v>128</v>
       </c>
       <c r="S39" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T39" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U39" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3268,7 +3277,7 @@
         <v>123</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D40" s="16" t="s">
         <v>141</v>
@@ -3276,7 +3285,7 @@
       <c r="E40" s="14"/>
       <c r="F40" s="17"/>
       <c r="G40" s="18" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H40" s="47">
         <v>21</v>
@@ -3284,31 +3293,35 @@
       <c r="I40" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J40" s="20"/>
+      <c r="J40" s="20" t="s">
+        <v>237</v>
+      </c>
       <c r="K40" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L40" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M40" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N40" s="23"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="O40" s="45"/>
       <c r="P40" s="47"/>
       <c r="Q40" s="34">
         <v>6</v>
       </c>
-      <c r="R40" s="34"/>
+      <c r="R40" s="34" t="s">
+        <v>128</v>
+      </c>
       <c r="S40" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T40" s="35" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="U40" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3319,7 +3332,7 @@
         <v>123</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D41" s="16" t="s">
         <v>141</v>
@@ -3327,7 +3340,7 @@
       <c r="E41" s="14"/>
       <c r="F41" s="17"/>
       <c r="G41" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H41" s="47">
         <v>22</v>
@@ -3335,31 +3348,35 @@
       <c r="I41" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J41" s="20"/>
+      <c r="J41" s="20" t="s">
+        <v>238</v>
+      </c>
       <c r="K41" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L41" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M41" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N41" s="23"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="O41" s="45"/>
       <c r="P41" s="47"/>
       <c r="Q41" s="34">
         <v>6</v>
       </c>
-      <c r="R41" s="34"/>
+      <c r="R41" s="34" t="s">
+        <v>128</v>
+      </c>
       <c r="S41" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T41" s="35" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="U41" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3370,7 +3387,7 @@
         <v>123</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D42" s="16" t="s">
         <v>141</v>
@@ -3378,7 +3395,7 @@
       <c r="E42" s="14"/>
       <c r="F42" s="17"/>
       <c r="G42" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H42" s="47">
         <v>23</v>
@@ -3386,31 +3403,35 @@
       <c r="I42" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J42" s="20"/>
+      <c r="J42" s="20" t="s">
+        <v>239</v>
+      </c>
       <c r="K42" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L42" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M42" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N42" s="23"/>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="O42" s="45"/>
       <c r="P42" s="47"/>
       <c r="Q42" s="34">
         <v>6</v>
       </c>
-      <c r="R42" s="34"/>
+      <c r="R42" s="34" t="s">
+        <v>128</v>
+      </c>
       <c r="S42" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T42" s="35" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="U42" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:21" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3421,10 +3442,10 @@
         <v>123</v>
       </c>
       <c r="C43" s="58" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="5"/>
@@ -3436,7 +3457,7 @@
       </c>
       <c r="I43" s="28"/>
       <c r="J43" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K43" s="29" t="s">
         <v>20</v>
@@ -3462,15 +3483,15 @@
         <v>127</v>
       </c>
       <c r="C44" s="58" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="5"/>
       <c r="G44" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H44" s="48">
         <v>25</v>
@@ -3479,7 +3500,7 @@
         <v>20</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K44" s="29" t="s">
         <v>20</v>
@@ -3505,7 +3526,7 @@
         <v>129</v>
       </c>
       <c r="T44" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U44" s="8" t="s">
         <v>131</v>
@@ -3519,15 +3540,15 @@
         <v>127</v>
       </c>
       <c r="C45" s="58" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="5"/>
       <c r="G45" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H45" s="48">
         <v>26</v>
@@ -3536,7 +3557,7 @@
         <v>20</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K45" s="29" t="s">
         <v>20</v>
@@ -3562,7 +3583,7 @@
         <v>129</v>
       </c>
       <c r="T45" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="U45" s="8" t="s">
         <v>131</v>

</xml_diff>